<commit_message>
add tiammao && xiaomi comments
</commit_message>
<xml_diff>
--- a/Comment/crawlcomments/info.xlsx
+++ b/Comment/crawlcomments/info.xlsx
@@ -8,20 +8,137 @@
   </bookViews>
   <sheets>
     <sheet name="jd" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="tb" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>chendong</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>chendong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+sku-data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>chendong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+comment-counts
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>chendong</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>chendong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+sellerId
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+  <si>
+    <t>573751869065</t>
+  </si>
+  <si>
+    <t>573881947497</t>
+  </si>
+  <si>
+    <t>576769538101</t>
+  </si>
+  <si>
+    <t>558867566371</t>
+  </si>
+  <si>
+    <t>574016715777</t>
+  </si>
+  <si>
+    <t>576313466920</t>
+  </si>
+  <si>
+    <t>578410957034</t>
+  </si>
+  <si>
+    <t>573735481083</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -29,6 +146,148 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -39,149 +298,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -192,187 +308,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,45 +499,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -436,26 +513,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,8 +535,67 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,153 +604,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,10 +1110,14 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -1477,23 +1603,118 @@
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>2616970884</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1714128138</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2633707274</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3077412435</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2755000148</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3991388630</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>4065459893</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>2277456896</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>